<commit_message>
treemap formatting matches scatterplot
</commit_message>
<xml_diff>
--- a/SchoolData.xlsx
+++ b/SchoolData.xlsx
@@ -222,7 +222,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -253,13 +256,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -284,14 +280,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -635,14 +630,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
-    <col min="4" max="9" width="10.83203125" style="4" customWidth="1"/>
+    <col min="4" max="9" width="10.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -675,1006 +670,1006 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3">
-        <v>0.52</v>
+        <v>0.52144999176141005</v>
       </c>
       <c r="D2" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.138375350140056</v>
       </c>
       <c r="E2" s="3">
-        <v>0.21</v>
+        <v>0.213049925852694</v>
       </c>
       <c r="F2" s="3">
-        <v>0.16</v>
+        <v>0.15901796012522701</v>
       </c>
       <c r="G2" s="3">
-        <v>0.66</v>
+        <v>0.65919743912198503</v>
       </c>
       <c r="H2" s="3">
-        <v>0.75</v>
+        <v>0.74507263810493196</v>
       </c>
       <c r="I2" s="3">
-        <v>0.65</v>
+        <v>0.64896562958136506</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>0.54</v>
+        <v>0.54040941113917296</v>
       </c>
       <c r="D3" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.8124418450086405E-2</v>
       </c>
       <c r="E3" s="3">
-        <v>0.25</v>
+        <v>0.24611192343480001</v>
       </c>
       <c r="F3" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.139505516416323</v>
       </c>
       <c r="G3" s="3">
-        <v>0.59</v>
+        <v>0.58592132505175998</v>
       </c>
       <c r="H3" s="3">
-        <v>0.78</v>
+        <v>0.78343399482312304</v>
       </c>
       <c r="I3" s="3">
-        <v>0.67</v>
+        <v>0.67215815485996699</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>0.38</v>
+        <v>0.37728459530026098</v>
       </c>
       <c r="D4" s="3">
-        <v>0.09</v>
+        <v>8.8120104438642294E-2</v>
       </c>
       <c r="E4" s="3">
-        <v>0.15</v>
+        <v>0.151436031331593</v>
       </c>
       <c r="F4" s="3">
-        <v>0.05</v>
+        <v>4.9608355091383803E-2</v>
       </c>
       <c r="G4" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.57142857142857095</v>
       </c>
       <c r="H4" s="3">
-        <v>0.91</v>
+        <v>0.90855457227138603</v>
       </c>
       <c r="I4" s="3">
-        <v>0.86</v>
+        <v>0.85806451612903201</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3">
-        <v>0.36</v>
+        <v>0.357594936708861</v>
       </c>
       <c r="D5" s="3">
-        <v>0.05</v>
+        <v>4.9367088607594901E-2</v>
       </c>
       <c r="E5" s="3">
-        <v>0.22</v>
+        <v>0.22088607594936699</v>
       </c>
       <c r="F5" s="3">
-        <v>0.04</v>
+        <v>4.05063291139241E-2</v>
       </c>
       <c r="G5" s="3">
-        <v>0.65</v>
+        <v>0.65102639296187703</v>
       </c>
       <c r="H5" s="3">
-        <v>0.9</v>
+        <v>0.90217391304347805</v>
       </c>
       <c r="I5" s="3">
-        <v>0.81</v>
+        <v>0.80714285714285705</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3">
-        <v>0.52</v>
+        <v>0.52194787379972596</v>
       </c>
       <c r="D6" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.7215363511659798E-2</v>
       </c>
       <c r="E6" s="3">
-        <v>0.23</v>
+        <v>0.229766803840878</v>
       </c>
       <c r="F6" s="3">
-        <v>0.04</v>
+        <v>4.4581618655692698E-2</v>
       </c>
       <c r="G6" s="3">
-        <v>0.6</v>
+        <v>0.59629629629629599</v>
       </c>
       <c r="H6" s="3">
-        <v>0.75</v>
+        <v>0.75226586102718995</v>
       </c>
       <c r="I6" s="3">
-        <v>0.69</v>
+        <v>0.68518518518518501</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3">
-        <v>0.68</v>
+        <v>0.67595818815330999</v>
       </c>
       <c r="D7" s="3">
-        <v>0.06</v>
+        <v>5.5749128919860599E-2</v>
       </c>
       <c r="E7" s="3">
-        <v>0.3</v>
+        <v>0.303135888501742</v>
       </c>
       <c r="F7" s="3">
-        <v>0.05</v>
+        <v>4.8780487804878099E-2</v>
       </c>
       <c r="G7" s="3">
-        <v>0.08</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H7" s="3">
-        <v>0.16</v>
+        <v>0.15702479338843001</v>
       </c>
       <c r="I7" s="3">
-        <v>0.15</v>
+        <v>0.14583333333333301</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3">
-        <v>0.6</v>
+        <v>0.59556378835375701</v>
       </c>
       <c r="D8" s="3">
-        <v>0.11</v>
+        <v>0.113090149140306</v>
       </c>
       <c r="E8" s="3">
-        <v>0.26</v>
+        <v>0.26223045502042402</v>
       </c>
       <c r="F8" s="3">
-        <v>0.16</v>
+        <v>0.16272442291251099</v>
       </c>
       <c r="G8" s="3">
-        <v>0.7</v>
+        <v>0.69519094766619505</v>
       </c>
       <c r="H8" s="3">
-        <v>0.76</v>
+        <v>0.76193282262816697</v>
       </c>
       <c r="I8" s="3">
-        <v>0.67</v>
+        <v>0.67450980392156901</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3">
-        <v>0.48</v>
+        <v>0.47899159663865498</v>
       </c>
       <c r="D9" s="3">
-        <v>0.08</v>
+        <v>7.5630252100840303E-2</v>
       </c>
       <c r="E9" s="3">
-        <v>0.32</v>
+        <v>0.31932773109243701</v>
       </c>
       <c r="F9" s="3">
-        <v>0.03</v>
+        <v>2.5210084033613401E-2</v>
       </c>
       <c r="G9" s="3">
-        <v>0.13</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="H9" s="3">
-        <v>0.46</v>
+        <v>0.46031746031746001</v>
       </c>
       <c r="I9" s="3">
         <v>0.42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3">
-        <v>0.47</v>
+        <v>0.46833333333333299</v>
       </c>
       <c r="D10" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.138333333333333</v>
       </c>
       <c r="E10" s="3">
-        <v>0.23</v>
+        <v>0.230833333333333</v>
       </c>
       <c r="F10" s="3">
-        <v>0.05</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="G10" s="3">
-        <v>0.65</v>
+        <v>0.64516129032258096</v>
       </c>
       <c r="H10" s="3">
-        <v>0.75</v>
+        <v>0.75084175084175098</v>
       </c>
       <c r="I10" s="3">
-        <v>0.64</v>
+        <v>0.63636363636363602</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3">
-        <v>0.64</v>
+        <v>0.63846767757382294</v>
       </c>
       <c r="D11" s="3">
-        <v>0.15</v>
+        <v>0.15323224261771701</v>
       </c>
       <c r="E11" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.282521947326417</v>
       </c>
       <c r="F11" s="3">
-        <v>0.09</v>
+        <v>8.9385474860335198E-2</v>
       </c>
       <c r="G11" s="3">
-        <v>0.82</v>
+        <v>0.819620253164557</v>
       </c>
       <c r="H11" s="3">
-        <v>0.71</v>
+        <v>0.71294117647058797</v>
       </c>
       <c r="I11" s="3">
-        <v>0.63</v>
+        <v>0.62662337662337697</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="3">
-        <v>0.16</v>
+        <v>0.16194331983805699</v>
       </c>
       <c r="D12" s="3">
-        <v>0.05</v>
+        <v>4.8582995951416998E-2</v>
       </c>
       <c r="E12" s="3">
-        <v>0.12</v>
+        <v>0.11740890688259099</v>
       </c>
       <c r="F12" s="3">
-        <v>0.02</v>
+        <v>1.6194331983805699E-2</v>
       </c>
       <c r="G12" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29032258064516098</v>
       </c>
       <c r="H12" s="3">
-        <v>0.41</v>
+        <v>0.41463414634146301</v>
       </c>
       <c r="I12" s="3">
-        <v>0.32</v>
+        <v>0.31818181818181801</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3">
-        <v>0.54</v>
+        <v>0.53609721229449603</v>
       </c>
       <c r="D13" s="3">
-        <v>0.09</v>
+        <v>9.1493924231593998E-2</v>
       </c>
       <c r="E13" s="3">
-        <v>0.25</v>
+        <v>0.24660471765546799</v>
       </c>
       <c r="F13" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>7.2194424588992098E-2</v>
       </c>
       <c r="G13" s="3">
-        <v>0.79</v>
+        <v>0.78571428571428603</v>
       </c>
       <c r="H13" s="3">
-        <v>0.83</v>
+        <v>0.82973621103117501</v>
       </c>
       <c r="I13" s="3">
-        <v>0.76</v>
+        <v>0.75845410628019305</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3">
-        <v>0.46</v>
+        <v>0.45615227736233899</v>
       </c>
       <c r="D14" s="3">
-        <v>0.13</v>
+        <v>0.13324269204622699</v>
       </c>
       <c r="E14" s="3">
-        <v>0.16</v>
+        <v>0.163834126444596</v>
       </c>
       <c r="F14" s="3">
-        <v>0.03</v>
+        <v>2.9911624745071402E-2</v>
       </c>
       <c r="G14" s="3">
-        <v>0.64</v>
+        <v>0.64213197969543101</v>
       </c>
       <c r="H14" s="3">
-        <v>0.82</v>
+        <v>0.824295010845987</v>
       </c>
       <c r="I14" s="3">
-        <v>0.77</v>
+        <v>0.77186311787072204</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="3">
-        <v>0.69</v>
+        <v>0.69344393898849299</v>
       </c>
       <c r="D15" s="3">
-        <v>0.11</v>
+        <v>0.114690928552315</v>
       </c>
       <c r="E15" s="3">
-        <v>0.37</v>
+        <v>0.369333690125769</v>
       </c>
       <c r="F15" s="3">
-        <v>0.22</v>
+        <v>0.21621621621621601</v>
       </c>
       <c r="G15" s="3">
-        <v>0.68</v>
+        <v>0.67709384460141298</v>
       </c>
       <c r="H15" s="3">
-        <v>0.63</v>
+        <v>0.62863070539419097</v>
       </c>
       <c r="I15" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.56621880998080598</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3">
-        <v>0.75</v>
+        <v>0.74761904761904796</v>
       </c>
       <c r="D16" s="3">
-        <v>0.19</v>
+        <v>0.192857142857143</v>
       </c>
       <c r="E16" s="3">
-        <v>0.38</v>
+        <v>0.38333333333333303</v>
       </c>
       <c r="F16" s="3">
-        <v>0.23</v>
+        <v>0.23095238095238099</v>
       </c>
       <c r="G16" s="3">
-        <v>0.09</v>
+        <v>9.3333333333333296E-2</v>
       </c>
       <c r="H16" s="3">
-        <v>0.64</v>
+        <v>0.64210526315789496</v>
       </c>
       <c r="I16" s="3">
-        <v>0.62</v>
+        <v>0.61728395061728403</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>0.73</v>
+        <v>0.733082706766917</v>
       </c>
       <c r="D17" s="3">
-        <v>0.09</v>
+        <v>9.3984962406015005E-2</v>
       </c>
       <c r="E17" s="3">
-        <v>0.53</v>
+        <v>0.52631578947368396</v>
       </c>
       <c r="F17" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.14285714285714299</v>
       </c>
       <c r="G17" s="3">
-        <v>0.53</v>
+        <v>0.53333333333333299</v>
       </c>
       <c r="H17" s="3">
-        <v>0.59</v>
+        <v>0.58823529411764697</v>
       </c>
       <c r="I17" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.57142857142857095</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="3">
-        <v>0.16</v>
+        <v>0.15925058548009399</v>
       </c>
       <c r="D18" s="3">
-        <v>0.05</v>
+        <v>5.15222482435597E-2</v>
       </c>
       <c r="E18" s="3">
-        <v>0.1</v>
+        <v>0.100702576112412</v>
       </c>
       <c r="F18" s="3">
-        <v>0</v>
+        <v>4.6838407494145199E-3</v>
       </c>
       <c r="G18" s="3">
-        <v>0.98</v>
+        <v>0.978494623655914</v>
       </c>
       <c r="H18" s="3">
-        <v>0.98</v>
+        <v>0.97938144329896903</v>
       </c>
       <c r="I18" s="3">
-        <v>0.92</v>
+        <v>0.91666666666666696</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="3">
-        <v>0.59</v>
+        <v>0.590425531914894</v>
       </c>
       <c r="D19" s="3">
-        <v>0.09</v>
+        <v>8.5106382978723402E-2</v>
       </c>
       <c r="E19" s="3">
-        <v>0.31</v>
+        <v>0.31382978723404298</v>
       </c>
       <c r="F19" s="3">
-        <v>0.04</v>
+        <v>3.7234042553191501E-2</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
       </c>
       <c r="H19" s="3">
-        <v>0.61</v>
+        <v>0.60714285714285698</v>
       </c>
       <c r="I19" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.54545454545454497</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="3">
-        <v>0.77</v>
+        <v>0.77155172413793105</v>
       </c>
       <c r="D20" s="3">
-        <v>0.16</v>
+        <v>0.163793103448276</v>
       </c>
       <c r="E20" s="3">
-        <v>0.37</v>
+        <v>0.37284482758620702</v>
       </c>
       <c r="F20" s="3">
-        <v>0.24</v>
+        <v>0.23706896551724099</v>
       </c>
       <c r="G20" s="3">
-        <v>0.9</v>
+        <v>0.89552238805970197</v>
       </c>
       <c r="H20" s="3">
-        <v>0.66</v>
+        <v>0.65517241379310298</v>
       </c>
       <c r="I20" s="3">
-        <v>0.62</v>
+        <v>0.62337662337662303</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="3">
-        <v>0.81</v>
+        <v>0.80738786279683405</v>
       </c>
       <c r="D21" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.14248021108179401</v>
       </c>
       <c r="E21" s="3">
-        <v>0.32</v>
+        <v>0.31662269129287601</v>
       </c>
       <c r="F21" s="3">
-        <v>0.1</v>
+        <v>0.10026385224274401</v>
       </c>
       <c r="G21" s="3">
-        <v>0.88</v>
+        <v>0.88405797101449302</v>
       </c>
       <c r="H21" s="3">
-        <v>0.82</v>
+        <v>0.81707317073170704</v>
       </c>
       <c r="I21" s="3">
-        <v>0.8</v>
+        <v>0.80281690140845097</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3">
-        <v>0.62</v>
+        <v>0.617942768754834</v>
       </c>
       <c r="D22" s="3">
-        <v>0.09</v>
+        <v>9.4354215003866995E-2</v>
       </c>
       <c r="E22" s="3">
-        <v>0.37</v>
+        <v>0.37432327919566899</v>
       </c>
       <c r="F22" s="3">
-        <v>0.08</v>
+        <v>8.1206496519721602E-2</v>
       </c>
       <c r="G22" s="3">
-        <v>0.63</v>
+        <v>0.625</v>
       </c>
       <c r="H22" s="3">
-        <v>0.64</v>
+        <v>0.63722397476340698</v>
       </c>
       <c r="I22" s="3">
-        <v>0.59</v>
+        <v>0.59009009009008995</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="3">
-        <v>0.47</v>
+        <v>0.46679197994987498</v>
       </c>
       <c r="D23" s="3">
-        <v>0.1</v>
+        <v>9.7744360902255606E-2</v>
       </c>
       <c r="E23" s="3">
-        <v>0.26</v>
+        <v>0.25877192982456099</v>
       </c>
       <c r="F23" s="3">
-        <v>0.04</v>
+        <v>4.13533834586466E-2</v>
       </c>
       <c r="G23" s="3">
-        <v>0.91</v>
+        <v>0.91304347826086996</v>
       </c>
       <c r="H23" s="3">
-        <v>0.65</v>
+        <v>0.65374677002584003</v>
       </c>
       <c r="I23" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.56097560975609795</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="3">
-        <v>0.87</v>
+        <v>0.87301587301587302</v>
       </c>
       <c r="D24" s="3">
-        <v>0.09</v>
+        <v>8.7301587301587297E-2</v>
       </c>
       <c r="E24" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.57936507936507897</v>
       </c>
       <c r="F24" s="3">
-        <v>0.09</v>
+        <v>8.7301587301587297E-2</v>
       </c>
       <c r="G24" s="3">
-        <v>0.11</v>
+        <v>0.114285714285714</v>
       </c>
       <c r="H24" s="3">
-        <v>0.25</v>
+        <v>0.246153846153846</v>
       </c>
       <c r="I24" s="3">
-        <v>0.26</v>
+        <v>0.25806451612903197</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="3">
-        <v>0.64</v>
+        <v>0.63855421686747005</v>
       </c>
       <c r="D25" s="3">
-        <v>0.16</v>
+        <v>0.156626506024096</v>
       </c>
       <c r="E25" s="3">
-        <v>0.49</v>
+        <v>0.49397590361445798</v>
       </c>
       <c r="F25" s="3">
-        <v>0.12</v>
+        <v>0.120481927710843</v>
       </c>
       <c r="G25" s="3">
-        <v>0.04</v>
+        <v>4.3478260869565202E-2</v>
       </c>
       <c r="H25" s="3">
-        <v>0.66</v>
+        <v>0.65625</v>
       </c>
       <c r="I25" s="3">
-        <v>0.65</v>
+        <v>0.64516129032258096</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="3">
-        <v>0.67</v>
+        <v>0.67375886524822703</v>
       </c>
       <c r="D26" s="3">
-        <v>0.08</v>
+        <v>7.8014184397163094E-2</v>
       </c>
       <c r="E26" s="3">
-        <v>0.33</v>
+        <v>0.32624113475177302</v>
       </c>
       <c r="F26" s="3">
-        <v>0.09</v>
+        <v>8.5106382978723402E-2</v>
       </c>
       <c r="G26" s="3">
-        <v>0.8</v>
+        <v>0.80357142857142905</v>
       </c>
       <c r="H26" s="3">
-        <v>0.79</v>
+        <v>0.78787878787878796</v>
       </c>
       <c r="I26" s="3">
-        <v>0.79</v>
+        <v>0.79245283018867896</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="3">
-        <v>0.52</v>
+        <v>0.521523298789767</v>
       </c>
       <c r="D27" s="3">
-        <v>0.12</v>
+        <v>0.121929125298935</v>
       </c>
       <c r="E27" s="3">
-        <v>0.21</v>
+        <v>0.208602072613958</v>
       </c>
       <c r="F27" s="3">
-        <v>0.18</v>
+        <v>0.17820131893615501</v>
       </c>
       <c r="G27" s="3">
-        <v>0.6</v>
+        <v>0.60217113665389499</v>
       </c>
       <c r="H27" s="3">
-        <v>0.79</v>
+        <v>0.78579003181336204</v>
       </c>
       <c r="I27" s="3">
-        <v>0.69</v>
+        <v>0.68842105263157904</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="3">
-        <v>0.67</v>
+        <v>0.673943334881561</v>
       </c>
       <c r="D28" s="3">
-        <v>0.18</v>
+        <v>0.18300046446818399</v>
       </c>
       <c r="E28" s="3">
-        <v>0.26</v>
+        <v>0.25870877844867601</v>
       </c>
       <c r="F28" s="3">
-        <v>0.16</v>
+        <v>0.16163492800743101</v>
       </c>
       <c r="G28" s="3">
-        <v>0.53</v>
+        <v>0.53235294117647103</v>
       </c>
       <c r="H28" s="3">
-        <v>0.7</v>
+        <v>0.69859813084112199</v>
       </c>
       <c r="I28" s="3">
-        <v>0.65</v>
+        <v>0.64687499999999998</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="3">
-        <v>0.33</v>
+        <v>0.33236151603498498</v>
       </c>
       <c r="D29" s="3">
-        <v>0.1</v>
+        <v>9.9125364431486895E-2</v>
       </c>
       <c r="E29" s="3">
-        <v>0.12</v>
+        <v>0.122448979591837</v>
       </c>
       <c r="F29" s="3">
-        <v>0.02</v>
+        <v>1.7492711370262402E-2</v>
       </c>
       <c r="G29" s="3">
-        <v>0.13</v>
+        <v>0.125</v>
       </c>
       <c r="H29" s="3">
         <v>0.62</v>
       </c>
       <c r="I29" s="3">
-        <v>0.54</v>
+        <v>0.54285714285714304</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="3">
-        <v>0.63</v>
+        <v>0.63087248322147604</v>
       </c>
       <c r="D30" s="3">
-        <v>0.1</v>
+        <v>0.10402684563758401</v>
       </c>
       <c r="E30" s="3">
-        <v>0.23</v>
+        <v>0.228187919463087</v>
       </c>
       <c r="F30" s="3">
-        <v>0.04</v>
+        <v>4.0268456375838903E-2</v>
       </c>
       <c r="G30" s="3">
-        <v>0.19</v>
+        <v>0.19298245614035101</v>
       </c>
       <c r="H30" s="3">
-        <v>0.33</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="I30" s="3">
-        <v>0.23</v>
+        <v>0.22666666666666699</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="3">
-        <v>0.36</v>
+        <v>0.358355091383812</v>
       </c>
       <c r="D31" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.6579634464751999E-2</v>
       </c>
       <c r="E31" s="3">
-        <v>0.15</v>
+        <v>0.152741514360313</v>
       </c>
       <c r="F31" s="3">
-        <v>0.05</v>
+        <v>5.3524804177545703E-2</v>
       </c>
       <c r="G31" s="3">
-        <v>0.59</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="H31" s="3">
-        <v>0.84</v>
+        <v>0.84117647058823497</v>
       </c>
       <c r="I31" s="3">
-        <v>0.76</v>
+        <v>0.75657894736842102</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="3">
-        <v>0.3</v>
+        <v>0.30118829981718498</v>
       </c>
       <c r="D32" s="3">
-        <v>0.1</v>
+        <v>9.5978062157221197E-2</v>
       </c>
       <c r="E32" s="3">
-        <v>0.11</v>
+        <v>0.10968921389396701</v>
       </c>
       <c r="F32" s="3">
-        <v>0.03</v>
+        <v>3.1992687385740397E-2</v>
       </c>
       <c r="G32" s="3">
-        <v>0.66</v>
+        <v>0.66139954853273097</v>
       </c>
       <c r="H32" s="3">
-        <v>0.9</v>
+        <v>0.90062111801242195</v>
       </c>
       <c r="I32" s="3">
-        <v>0.85</v>
+        <v>0.85142857142857098</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="3">
-        <v>0.35</v>
+        <v>0.34609646941819999</v>
       </c>
       <c r="D33" s="3">
-        <v>0.09</v>
+        <v>8.6524117354549998E-2</v>
       </c>
       <c r="E33" s="3">
-        <v>0.16</v>
+        <v>0.15514669318746899</v>
       </c>
       <c r="F33" s="3">
-        <v>0.06</v>
+        <v>5.9671805072103401E-2</v>
       </c>
       <c r="G33" s="3">
-        <v>0.7</v>
+        <v>0.70025188916876602</v>
       </c>
       <c r="H33" s="3">
-        <v>0.84</v>
+        <v>0.83651804670912999</v>
       </c>
       <c r="I33" s="3">
-        <v>0.77</v>
+        <v>0.772486772486772</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="3">
-        <v>0.54</v>
+        <v>0.53599839561467999</v>
       </c>
       <c r="D34" s="3">
-        <v>0.18</v>
+        <v>0.178019921117722</v>
       </c>
       <c r="E34" s="3">
-        <v>0.21</v>
+        <v>0.211778862223411</v>
       </c>
       <c r="F34" s="3">
-        <v>0.16</v>
+        <v>0.16337990507386899</v>
       </c>
       <c r="G34" s="3">
         <v>0.5</v>
       </c>
       <c r="H34" s="3">
-        <v>0.77</v>
+        <v>0.76923076923076905</v>
       </c>
       <c r="I34" s="3">
-        <v>0.7</v>
+        <v>0.69834087481146301</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="3">
-        <v>0.33</v>
+        <v>0.33402061855670101</v>
       </c>
       <c r="D35" s="3">
-        <v>0.08</v>
+        <v>8.1099656357388306E-2</v>
       </c>
       <c r="E35" s="3">
-        <v>0.2</v>
+        <v>0.19725085910652901</v>
       </c>
       <c r="F35" s="3">
-        <v>0.06</v>
+        <v>5.9106529209621998E-2</v>
       </c>
       <c r="G35" s="3">
-        <v>0.59</v>
+        <v>0.58983050847457597</v>
       </c>
       <c r="H35" s="3">
-        <v>0.88</v>
+        <v>0.88328075709779197</v>
       </c>
       <c r="I35" s="3">
-        <v>0.84</v>
+        <v>0.83673469387755095</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>46</v>
       </c>
       <c r="C36" s="3">
-        <v>0.37</v>
+        <v>0.36885245901639302</v>
       </c>
       <c r="D36" s="3">
-        <v>0.18</v>
+        <v>0.18032786885245899</v>
       </c>
       <c r="E36" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5573770491803296E-2</v>
       </c>
       <c r="F36" s="3">
         <v>0</v>
@@ -1683,561 +1678,561 @@
         <v>0</v>
       </c>
       <c r="H36" s="3">
-        <v>0.76</v>
+        <v>0.75609756097560998</v>
       </c>
       <c r="I36" s="3">
-        <v>0.69</v>
+        <v>0.69230769230769196</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="3">
-        <v>0.47</v>
+        <v>0.47295208655332299</v>
       </c>
       <c r="D37" s="3">
-        <v>0.17</v>
+        <v>0.173879443585781</v>
       </c>
       <c r="E37" s="3">
-        <v>0.16</v>
+        <v>0.160741885625966</v>
       </c>
       <c r="F37" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.6460587326120604E-2</v>
       </c>
       <c r="G37" s="3">
-        <v>0.59</v>
+        <v>0.58935361216729998</v>
       </c>
       <c r="H37" s="3">
-        <v>0.87</v>
+        <v>0.86643835616438403</v>
       </c>
       <c r="I37" s="3">
-        <v>0.79</v>
+        <v>0.78571428571428603</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="3">
-        <v>0.63</v>
+        <v>0.62774829416224398</v>
       </c>
       <c r="D38" s="3">
-        <v>0.33</v>
+        <v>0.33131159969674001</v>
       </c>
       <c r="E38" s="3">
-        <v>0.19</v>
+        <v>0.18953752843062899</v>
       </c>
       <c r="F38" s="3">
-        <v>0.1</v>
+        <v>0.104624715693707</v>
       </c>
       <c r="G38" s="3">
-        <v>0.52</v>
+        <v>0.522088353413655</v>
       </c>
       <c r="H38" s="3">
-        <v>0.77</v>
+        <v>0.76948051948051899</v>
       </c>
       <c r="I38" s="3">
-        <v>0.75</v>
+        <v>0.74576271186440701</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="3">
-        <v>0.4</v>
+        <v>0.402426457721696</v>
       </c>
       <c r="D39" s="3">
-        <v>0.17</v>
+        <v>0.170940835650263</v>
       </c>
       <c r="E39" s="3">
-        <v>0.13</v>
+        <v>0.12596970816401901</v>
       </c>
       <c r="F39" s="3">
-        <v>0.12</v>
+        <v>0.1166760640056</v>
       </c>
       <c r="G39" s="3">
-        <v>0.76</v>
+        <v>0.75545058139534904</v>
       </c>
       <c r="H39" s="3">
-        <v>0.75</v>
+        <v>0.75477897252090798</v>
       </c>
       <c r="I39" s="3">
-        <v>0.65</v>
+        <v>0.64866468842729996</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
         <v>47</v>
       </c>
       <c r="C40" s="3">
-        <v>0.17</v>
+        <v>0.174317617866005</v>
       </c>
       <c r="D40" s="3">
-        <v>0.05</v>
+        <v>5.2729528535980098E-2</v>
       </c>
       <c r="E40" s="3">
-        <v>0.1</v>
+        <v>9.9255583126550903E-2</v>
       </c>
       <c r="F40" s="3">
-        <v>0.02</v>
+        <v>1.86104218362283E-2</v>
       </c>
       <c r="G40" s="3">
-        <v>0.64</v>
+        <v>0.64242424242424201</v>
       </c>
       <c r="H40" s="3">
-        <v>0.88</v>
+        <v>0.87921348314606695</v>
       </c>
       <c r="I40" s="3">
-        <v>0.75</v>
+        <v>0.75280898876404501</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.57561361836896296</v>
       </c>
       <c r="D41" s="3">
-        <v>0.2</v>
+        <v>0.201900237529691</v>
       </c>
       <c r="E41" s="3">
-        <v>0.24</v>
+        <v>0.24386381631037199</v>
       </c>
       <c r="F41" s="3">
-        <v>0.12</v>
+        <v>0.120348376880443</v>
       </c>
       <c r="G41" s="3">
-        <v>0.71</v>
+        <v>0.70612244897959198</v>
       </c>
       <c r="H41" s="3">
-        <v>0.81</v>
+        <v>0.81338028169014098</v>
       </c>
       <c r="I41" s="3">
-        <v>0.76</v>
+        <v>0.76331360946745597</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="3">
-        <v>0.67</v>
+        <v>0.667439165701043</v>
       </c>
       <c r="D42" s="3">
-        <v>0.37</v>
+        <v>0.367323290845886</v>
       </c>
       <c r="E42" s="3">
-        <v>0.1</v>
+        <v>0.101969872537659</v>
       </c>
       <c r="F42" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9524913093858595E-2</v>
       </c>
       <c r="G42" s="3">
-        <v>0.66</v>
+        <v>0.65853658536585402</v>
       </c>
       <c r="H42" s="3">
-        <v>0.79</v>
+        <v>0.78947368421052599</v>
       </c>
       <c r="I42" s="3">
-        <v>0.79</v>
+        <v>0.79194630872483196</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="3">
-        <v>0.64</v>
+        <v>0.64363636363636401</v>
       </c>
       <c r="D43" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.27636363636363598</v>
       </c>
       <c r="E43" s="3">
-        <v>0.09</v>
+        <v>8.7272727272727293E-2</v>
       </c>
       <c r="F43" s="3">
-        <v>0.17</v>
+        <v>0.17309090909090899</v>
       </c>
       <c r="G43" s="3">
-        <v>0.78</v>
+        <v>0.77551020408163296</v>
       </c>
       <c r="H43" s="3">
-        <v>0.78</v>
+        <v>0.77586206896551702</v>
       </c>
       <c r="I43" s="3">
-        <v>0.76</v>
+        <v>0.76449275362318803</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="3">
-        <v>0.37</v>
+        <v>0.37378048780487799</v>
       </c>
       <c r="D44" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29329268292682897</v>
       </c>
       <c r="E44" s="3">
-        <v>0.08</v>
+        <v>8.10975609756098E-2</v>
       </c>
       <c r="F44" s="3">
-        <v>0.06</v>
+        <v>6.0975609756097601E-2</v>
       </c>
       <c r="G44" s="3">
-        <v>0.85</v>
+        <v>0.84766584766584796</v>
       </c>
       <c r="H44" s="3">
-        <v>0.87</v>
+        <v>0.87389380530973404</v>
       </c>
       <c r="I44" s="3">
-        <v>0.81</v>
+        <v>0.81443298969072198</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="3">
-        <v>0.34</v>
+        <v>0.33789954337899503</v>
       </c>
       <c r="D45" s="3">
-        <v>0.11</v>
+        <v>0.106849315068493</v>
       </c>
       <c r="E45" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.13698630136986301</v>
       </c>
       <c r="F45" s="3">
-        <v>0.06</v>
+        <v>6.4840182648401801E-2</v>
       </c>
       <c r="G45" s="3">
-        <v>0.74</v>
+        <v>0.74157303370786498</v>
       </c>
       <c r="H45" s="3">
-        <v>0.76</v>
+        <v>0.763636363636364</v>
       </c>
       <c r="I45" s="3">
-        <v>0.7</v>
+        <v>0.69696969696969702</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>49</v>
       </c>
       <c r="C46" s="3">
-        <v>0.9</v>
+        <v>0.90405117270788904</v>
       </c>
       <c r="D46" s="3">
-        <v>0.45</v>
+        <v>0.44776119402985098</v>
       </c>
       <c r="E46" s="3">
-        <v>0.23</v>
+        <v>0.228144989339019</v>
       </c>
       <c r="F46" s="3">
-        <v>0.08</v>
+        <v>7.6759061833688705E-2</v>
       </c>
       <c r="G46" s="3">
         <v>0.2</v>
       </c>
       <c r="H46" s="3">
-        <v>0.04</v>
+        <v>4.0201005025125601E-2</v>
       </c>
       <c r="I46" s="3">
         <v>0.04</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>50</v>
       </c>
       <c r="C47" s="3">
-        <v>0.6</v>
+        <v>0.60119047619047605</v>
       </c>
       <c r="D47" s="3">
-        <v>0.31</v>
+        <v>0.30952380952380998</v>
       </c>
       <c r="E47" s="3">
-        <v>0.16</v>
+        <v>0.160714285714286</v>
       </c>
       <c r="F47" s="3">
-        <v>0.08</v>
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="G47" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.28571428571428598</v>
       </c>
       <c r="H47" s="3">
-        <v>0.31</v>
+        <v>0.31395348837209303</v>
       </c>
       <c r="I47" s="3">
-        <v>0.23</v>
+        <v>0.230769230769231</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="3">
-        <v>0.31</v>
+        <v>0.30708661417322802</v>
       </c>
       <c r="D48" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.13560804899387599</v>
       </c>
       <c r="E48" s="3">
-        <v>0.11</v>
+        <v>0.10761154855643</v>
       </c>
       <c r="F48" s="3">
-        <v>0.06</v>
+        <v>6.2117235345581799E-2</v>
       </c>
       <c r="G48" s="3">
-        <v>0.94</v>
+        <v>0.93916349809885902</v>
       </c>
       <c r="H48" s="3">
-        <v>0.92</v>
+        <v>0.91575091575091605</v>
       </c>
       <c r="I48" s="3">
-        <v>0.87</v>
+        <v>0.87356321839080497</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
         <v>52</v>
       </c>
       <c r="C49" s="3">
-        <v>0.25</v>
+        <v>0.25454545454545502</v>
       </c>
       <c r="D49" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>7.2727272727272696E-2</v>
       </c>
       <c r="E49" s="3">
-        <v>0.08</v>
+        <v>7.5757575757575801E-2</v>
       </c>
       <c r="F49" s="3">
         <v>0</v>
       </c>
       <c r="G49" s="3">
-        <v>0.1</v>
+        <v>9.8039215686274495E-2</v>
       </c>
       <c r="H49" s="3">
-        <v>0.51</v>
+        <v>0.50746268656716398</v>
       </c>
       <c r="I49" s="3">
-        <v>0.17</v>
+        <v>0.173913043478261</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
         <v>42</v>
       </c>
       <c r="C50" s="3">
-        <v>0.76</v>
+        <v>0.75619834710743805</v>
       </c>
       <c r="D50" s="3">
-        <v>0.51</v>
+        <v>0.51239669421487599</v>
       </c>
       <c r="E50" s="3">
-        <v>0.13</v>
+        <v>0.12603305785124</v>
       </c>
       <c r="F50" s="3">
-        <v>0.21</v>
+        <v>0.206611570247934</v>
       </c>
       <c r="G50" s="3">
-        <v>0.68</v>
+        <v>0.67708333333333304</v>
       </c>
       <c r="H50" s="3">
-        <v>0.79</v>
+        <v>0.78888888888888897</v>
       </c>
       <c r="I50" s="3">
-        <v>0.81</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.14310246136233501</v>
       </c>
       <c r="D51" s="3">
-        <v>0.06</v>
+        <v>5.6096164854035499E-2</v>
       </c>
       <c r="E51" s="3">
-        <v>0.09</v>
+        <v>8.5861476817401305E-2</v>
       </c>
       <c r="F51" s="3">
-        <v>0.03</v>
+        <v>2.5758443045220399E-2</v>
       </c>
       <c r="G51" s="3">
-        <v>0.97</v>
+        <v>0.96658097686375299</v>
       </c>
       <c r="H51" s="3">
-        <v>0.9</v>
+        <v>0.89663461538461497</v>
       </c>
       <c r="I51" s="3">
-        <v>0.79</v>
+        <v>0.78823529411764703</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="s">
         <v>54</v>
       </c>
       <c r="C52" s="3">
-        <v>0.18</v>
+        <v>0.17894736842105299</v>
       </c>
       <c r="D52" s="3">
-        <v>0.06</v>
+        <v>6.3157894736842093E-2</v>
       </c>
       <c r="E52" s="3">
-        <v>0.05</v>
+        <v>4.5614035087719301E-2</v>
       </c>
       <c r="F52" s="3">
-        <v>0</v>
+        <v>3.5087719298245602E-3</v>
       </c>
       <c r="G52" s="3">
         <v>1</v>
       </c>
       <c r="H52" s="3">
-        <v>0.89</v>
+        <v>0.88524590163934402</v>
       </c>
       <c r="I52" s="3">
-        <v>0.77</v>
+        <v>0.77272727272727304</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" t="s">
         <v>55</v>
       </c>
       <c r="C53" s="3">
-        <v>0.38</v>
+        <v>0.38351983723296001</v>
       </c>
       <c r="D53" s="3">
-        <v>0.16</v>
+        <v>0.163784333672431</v>
       </c>
       <c r="E53" s="3">
-        <v>0.13</v>
+        <v>0.128179043743642</v>
       </c>
       <c r="F53" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.7141403865717195E-2</v>
       </c>
       <c r="G53" s="3">
-        <v>0.59</v>
+        <v>0.58888888888888902</v>
       </c>
       <c r="H53" s="3">
-        <v>0.83</v>
+        <v>0.82692307692307698</v>
       </c>
       <c r="I53" s="3">
-        <v>0.75</v>
+        <v>0.75454545454545496</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="A54" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="3">
-        <v>0.81</v>
+        <v>0.80711864406779699</v>
       </c>
       <c r="D54" s="3">
-        <v>0.21</v>
+        <v>0.21220338983050799</v>
       </c>
       <c r="E54" s="3">
-        <v>0.27</v>
+        <v>0.26983050847457601</v>
       </c>
       <c r="F54" s="3">
-        <v>0.41</v>
+        <v>0.406440677966102</v>
       </c>
       <c r="G54" s="3">
-        <v>0.46</v>
+        <v>0.462686567164179</v>
       </c>
       <c r="H54" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.551219512195122</v>
       </c>
       <c r="I54" s="3">
-        <v>0.51</v>
+        <v>0.51162790697674398</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="s">
         <v>43</v>
       </c>
       <c r="C55" s="3">
-        <v>0.75</v>
+        <v>0.74801362088535694</v>
       </c>
       <c r="D55" s="3">
-        <v>0.21</v>
+        <v>0.207718501702611</v>
       </c>
       <c r="E55" s="3">
-        <v>0.25</v>
+        <v>0.24744608399546</v>
       </c>
       <c r="F55" s="3">
-        <v>0.31</v>
+        <v>0.31214528944381398</v>
       </c>
       <c r="G55" s="3">
-        <v>0.46</v>
+        <v>0.462686567164179</v>
       </c>
       <c r="H55" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.551219512195122</v>
       </c>
       <c r="I55" s="3">
-        <v>0.51</v>
+        <v>0.51162790697674398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>